<commit_message>
simple changes to styling
</commit_message>
<xml_diff>
--- a/data/tomorrow_gasprices_canadiancities_latlng.xlsx
+++ b/data/tomorrow_gasprices_canadiancities_latlng.xlsx
@@ -503,17 +503,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>152.9</t>
+          <t>146.9</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>182.9 ⮟ -5</t>
+          <t>176.9 ⮟ -6</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>197.9 ⮟ -2</t>
+          <t>191.9 ⮟ -4</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>1.53</v>
+        <v>1.47</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -545,11 +545,11 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>⮟ -5</t>
+          <t>⮟ -6</t>
         </is>
       </c>
     </row>
@@ -561,17 +561,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>167.9</t>
+          <t>161.9</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>191.9 ⮟ -5</t>
+          <t>185.9 ⮟ -6</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>238.9 ⮟ -2</t>
+          <t>215.9 ⮟ -5</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -595,7 +595,7 @@
         </is>
       </c>
       <c r="I3" t="n">
-        <v>1.68</v>
+        <v>1.62</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -603,11 +603,11 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>⮟ -5</t>
+          <t>⮟ -6</t>
         </is>
       </c>
     </row>
@@ -619,17 +619,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>169.9</t>
+          <t>163.9</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>191.9 ⮟ -2</t>
+          <t>187.9 ⮟ -5</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>219.9 n/c</t>
+          <t>216.9 ⮟ -5</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -653,7 +653,7 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>1.7</v>
+        <v>1.64</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -661,11 +661,11 @@
         </is>
       </c>
       <c r="K4" t="n">
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>⮟ -2</t>
+          <t>⮟ -5</t>
         </is>
       </c>
     </row>
@@ -677,17 +677,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>136.9</t>
+          <t>127.9</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>161.9 n/c</t>
+          <t>152.9 ⮟ -5</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>172.9 n/c</t>
+          <t>174.9 ⮟ -5</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -711,19 +711,19 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>1.37</v>
+        <v>1.28</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -5</t>
         </is>
       </c>
     </row>
@@ -735,17 +735,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>151.9</t>
+          <t>145.9</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>181.9 ⮟ -5</t>
+          <t>175.9 ⮟ -6</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>197.9 ⮟ -2</t>
+          <t>191.9 ⮟ -4</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -769,7 +769,7 @@
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1.52</v>
+        <v>1.46</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -777,11 +777,11 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>⮟ -5</t>
+          <t>⮟ -6</t>
         </is>
       </c>
     </row>
@@ -793,17 +793,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>152.9</t>
+          <t>146.9</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>182.9 ⮟ -5</t>
+          <t>176.9 ⮟ -6</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>197.9 ⮟ -2</t>
+          <t>191.9 ⮟ -4</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -827,7 +827,7 @@
         </is>
       </c>
       <c r="I7" t="n">
-        <v>1.53</v>
+        <v>1.47</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -835,11 +835,11 @@
         </is>
       </c>
       <c r="K7" t="n">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>⮟ -5</t>
+          <t>⮟ -6</t>
         </is>
       </c>
     </row>
@@ -851,17 +851,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>177.2</t>
+          <t>164.1</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>186.3 n/c</t>
+          <t>173.2 n/c</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>237.8 n/c</t>
+          <t>266.0 n/c</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -885,7 +885,7 @@
         </is>
       </c>
       <c r="I8" t="n">
-        <v>1.77</v>
+        <v>1.64</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -909,17 +909,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>157.9</t>
+          <t>148.9</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>182.9 n/c</t>
+          <t>174.9 ⮟ -5</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>220.9 n/c</t>
+          <t>205.9 ⮟ -6</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -943,19 +943,19 @@
         </is>
       </c>
       <c r="I9" t="n">
-        <v>1.58</v>
+        <v>1.49</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -6</t>
         </is>
       </c>
     </row>
@@ -967,17 +967,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>136.9</t>
+          <t>125.9</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>161.9 n/c</t>
+          <t>152.9 ⮟ -5</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>174.9 n/c</t>
+          <t>169.9 ⮟ -5</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1001,19 +1001,19 @@
         </is>
       </c>
       <c r="I10" t="n">
-        <v>1.37</v>
+        <v>1.26</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -5</t>
         </is>
       </c>
     </row>
@@ -1025,17 +1025,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>167.9</t>
+          <t>160.9</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>175.6 n/c</t>
+          <t>168.6 n/c</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>262.3 n/c</t>
+          <t>269.3 n/c</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1059,7 +1059,7 @@
         </is>
       </c>
       <c r="I11" t="n">
-        <v>1.68</v>
+        <v>1.61</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1083,17 +1083,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>152.9</t>
+          <t>146.9</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>182.9 ⮟ -5</t>
+          <t>176.9 ⮟ -6</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>197.9 ⮟ -2</t>
+          <t>191.9 ⮟ -4</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1117,7 +1117,7 @@
         </is>
       </c>
       <c r="I12" t="n">
-        <v>1.53</v>
+        <v>1.47</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1125,11 +1125,11 @@
         </is>
       </c>
       <c r="K12" t="n">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>⮟ -5</t>
+          <t>⮟ -6</t>
         </is>
       </c>
     </row>
@@ -1141,17 +1141,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>157.7</t>
+          <t>156.1</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>166.7 ⮟ -4</t>
+          <t>165.3 n/c</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>248.5 ⮟ -10</t>
+          <t>245.5 n/c</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1175,19 +1175,19 @@
         </is>
       </c>
       <c r="I13" t="n">
-        <v>1.58</v>
+        <v>1.56</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>⮟</t>
+          <t>n/c</t>
         </is>
       </c>
       <c r="K13" t="n">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>⮟ -4</t>
+          <t>n/c</t>
         </is>
       </c>
     </row>
@@ -1199,17 +1199,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>152.9</t>
+          <t>146.9</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>182.9 ⮟ -5</t>
+          <t>176.9 ⮟ -6</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>197.9 ⮟ -2</t>
+          <t>191.9 ⮟ -4</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1233,7 +1233,7 @@
         </is>
       </c>
       <c r="I14" t="n">
-        <v>1.53</v>
+        <v>1.47</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1241,11 +1241,11 @@
         </is>
       </c>
       <c r="K14" t="n">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>⮟ -5</t>
+          <t>⮟ -6</t>
         </is>
       </c>
     </row>
@@ -1257,17 +1257,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>175.9</t>
+          <t>165.9</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>197.9 n/c</t>
+          <t>187.9 ⮟ -4</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>205.9 n/c</t>
+          <t>201.9 ⮟ -4</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1291,19 +1291,19 @@
         </is>
       </c>
       <c r="I15" t="n">
-        <v>1.76</v>
+        <v>1.66</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -4</t>
         </is>
       </c>
     </row>
@@ -1315,17 +1315,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>175.9</t>
+          <t>165.9</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>197.9 n/c</t>
+          <t>187.9 ⮟ -4</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>205.9 n/c</t>
+          <t>201.9 ⮟ -4</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1349,19 +1349,19 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>1.76</v>
+        <v>1.66</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K16" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -4</t>
         </is>
       </c>
     </row>
@@ -1373,17 +1373,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>152.9</t>
+          <t>146.9</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>174.9 ⮟ -5</t>
+          <t>168.9 ⮟ -6</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>214.9 n/c</t>
+          <t>198.9 ⮟ -6</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1407,7 +1407,7 @@
         </is>
       </c>
       <c r="I17" t="n">
-        <v>1.53</v>
+        <v>1.47</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1415,11 +1415,11 @@
         </is>
       </c>
       <c r="K17" t="n">
-        <v>-2</v>
+        <v>-6</v>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>⮟ -2</t>
+          <t>⮟ -6</t>
         </is>
       </c>
     </row>
@@ -1431,17 +1431,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>151.9</t>
+          <t>145.9</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>181.9 ⮟ -5</t>
+          <t>175.9 ⮟ -6</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>197.9 ⮟ -2</t>
+          <t>191.9 ⮟ -4</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1465,7 +1465,7 @@
         </is>
       </c>
       <c r="I18" t="n">
-        <v>1.52</v>
+        <v>1.46</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1473,11 +1473,11 @@
         </is>
       </c>
       <c r="K18" t="n">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>⮟ -5</t>
+          <t>⮟ -6</t>
         </is>
       </c>
     </row>
@@ -1489,17 +1489,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>151.9</t>
+          <t>146.9</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>181.9 ⮟ -6</t>
+          <t>176.9 ⮟ -5</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>197.9 ⮟ -2</t>
+          <t>191.9 ⮟ -4</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1523,7 +1523,7 @@
         </is>
       </c>
       <c r="I19" t="n">
-        <v>1.52</v>
+        <v>1.47</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1531,11 +1531,11 @@
         </is>
       </c>
       <c r="K19" t="n">
-        <v>-6</v>
+        <v>-5</v>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>⮟ -6</t>
+          <t>⮟ -5</t>
         </is>
       </c>
     </row>
@@ -1547,17 +1547,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>152.9</t>
+          <t>146.9</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>182.9 ⮟ -5</t>
+          <t>176.9 ⮟ -6</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>197.9 ⮟ -2</t>
+          <t>191.9 ⮟ -4</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1581,7 +1581,7 @@
         </is>
       </c>
       <c r="I20" t="n">
-        <v>1.53</v>
+        <v>1.47</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1589,11 +1589,11 @@
         </is>
       </c>
       <c r="K20" t="n">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>⮟ -5</t>
+          <t>⮟ -6</t>
         </is>
       </c>
     </row>
@@ -1605,12 +1605,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>168.8</t>
+          <t>160.8</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>177.5 n/c</t>
+          <t>168.5 n/c</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1639,7 +1639,7 @@
         </is>
       </c>
       <c r="I21" t="n">
-        <v>1.69</v>
+        <v>1.61</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1663,17 +1663,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>152.9</t>
+          <t>146.9</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>182.9 ⮟ -5</t>
+          <t>176.9 ⮟ -6</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>197.9 ⮟ -2</t>
+          <t>191.9 ⮟ -4</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1697,7 +1697,7 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>1.53</v>
+        <v>1.47</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1705,11 +1705,11 @@
         </is>
       </c>
       <c r="K22" t="n">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>⮟ -5</t>
+          <t>⮟ -6</t>
         </is>
       </c>
     </row>
@@ -1721,17 +1721,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>152.9</t>
+          <t>146.9</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>182.9 ⮟ -5</t>
+          <t>176.9 ⮟ -6</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>197.9 ⮟ -2</t>
+          <t>191.9 ⮟ -4</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1755,7 +1755,7 @@
         </is>
       </c>
       <c r="I23" t="n">
-        <v>1.53</v>
+        <v>1.47</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1763,11 +1763,11 @@
         </is>
       </c>
       <c r="K23" t="n">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>⮟ -5</t>
+          <t>⮟ -6</t>
         </is>
       </c>
     </row>
@@ -1779,17 +1779,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>151.9</t>
+          <t>145.9</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>181.9 ⮟ -5</t>
+          <t>175.9 ⮟ -6</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>197.9 ⮟ -2</t>
+          <t>191.9 ⮟ -4</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1813,7 +1813,7 @@
         </is>
       </c>
       <c r="I24" t="n">
-        <v>1.52</v>
+        <v>1.46</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1821,11 +1821,11 @@
         </is>
       </c>
       <c r="K24" t="n">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>⮟ -5</t>
+          <t>⮟ -6</t>
         </is>
       </c>
     </row>
@@ -1837,17 +1837,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>152.9</t>
+          <t>146.9</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>199.9 ⮟ -5</t>
+          <t>193.9 ⮟ -6</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>209.9 ⮟ -2</t>
+          <t>204.9 ⮟ -5</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1871,7 +1871,7 @@
         </is>
       </c>
       <c r="I25" t="n">
-        <v>1.53</v>
+        <v>1.47</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -1879,11 +1879,11 @@
         </is>
       </c>
       <c r="K25" t="n">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>⮟ -5</t>
+          <t>⮟ -6</t>
         </is>
       </c>
     </row>
@@ -1895,17 +1895,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>157.9</t>
+          <t>140.9</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>186.9 n/c</t>
+          <t>165.9 ⮟ -3</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>215.9 n/c</t>
+          <t>196.9 ⮟ -3</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1929,19 +1929,19 @@
         </is>
       </c>
       <c r="I26" t="n">
-        <v>1.58</v>
+        <v>1.41</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K26" t="n">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -3</t>
         </is>
       </c>
     </row>
@@ -1953,17 +1953,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>175.9</t>
+          <t>165.9</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>197.9 n/c</t>
+          <t>187.9 ⮟ -4</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>211.9 n/c</t>
+          <t>195.9 ⮟ -4</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1987,19 +1987,19 @@
         </is>
       </c>
       <c r="I27" t="n">
-        <v>1.76</v>
+        <v>1.66</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K27" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -4</t>
         </is>
       </c>
     </row>
@@ -2011,17 +2011,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>169.9</t>
+          <t>165.9</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>191.9 ⮟ -5</t>
+          <t>187.9 ⮟ -6</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>231.9 ⮟ -3</t>
+          <t>215.9 ⮟ -4</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -2045,7 +2045,7 @@
         </is>
       </c>
       <c r="I28" t="n">
-        <v>1.7</v>
+        <v>1.66</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2053,11 +2053,11 @@
         </is>
       </c>
       <c r="K28" t="n">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>⮟ -5</t>
+          <t>⮟ -6</t>
         </is>
       </c>
     </row>
@@ -2069,17 +2069,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>155.9</t>
+          <t>147.9</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>179.9 n/c</t>
+          <t>170.9 ⮟ -7</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>199.9 n/c</t>
+          <t>197.9 ⮟ -2</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -2103,19 +2103,19 @@
         </is>
       </c>
       <c r="I29" t="n">
-        <v>1.56</v>
+        <v>1.48</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K29" t="n">
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -6</t>
         </is>
       </c>
     </row>
@@ -2127,17 +2127,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>155.9</t>
+          <t>147.9</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>179.9 n/c</t>
+          <t>170.9 ⮟ -7</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>199.9 n/c</t>
+          <t>197.9 ⮟ -2</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -2161,19 +2161,19 @@
         </is>
       </c>
       <c r="I30" t="n">
-        <v>1.56</v>
+        <v>1.48</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K30" t="n">
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -6</t>
         </is>
       </c>
     </row>
@@ -2185,17 +2185,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>152.9</t>
+          <t>146.9</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>182.9 ⮟ -5</t>
+          <t>176.9 ⮟ -6</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>197.9 ⮟ -2</t>
+          <t>191.9 ⮟ -4</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -2219,7 +2219,7 @@
         </is>
       </c>
       <c r="I31" t="n">
-        <v>1.53</v>
+        <v>1.47</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -2227,11 +2227,11 @@
         </is>
       </c>
       <c r="K31" t="n">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>⮟ -5</t>
+          <t>⮟ -6</t>
         </is>
       </c>
     </row>
@@ -2243,17 +2243,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>167.9</t>
+          <t>160.9</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>175.7 n/c</t>
+          <t>168.7 n/c</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>258.3 n/c</t>
+          <t>264.3 n/c</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -2277,7 +2277,7 @@
         </is>
       </c>
       <c r="I32" t="n">
-        <v>1.68</v>
+        <v>1.61</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -2301,17 +2301,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>167.1</t>
+          <t>169.4</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>173.1 n/c</t>
+          <t>175.4 n/c</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>270.7 n/c</t>
+          <t>272.7 n/c</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -2335,7 +2335,7 @@
         </is>
       </c>
       <c r="I33" t="n">
-        <v>1.67</v>
+        <v>1.69</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -2359,17 +2359,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>157.9</t>
+          <t>153.2</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>187.6 ⮟ -2</t>
+          <t>182.8 ⮟ -4</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>223.9 ⮟ -1</t>
+          <t>202.9 ⮟ -3</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -2393,7 +2393,7 @@
         </is>
       </c>
       <c r="I34" t="n">
-        <v>1.58</v>
+        <v>1.53</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -2401,11 +2401,11 @@
         </is>
       </c>
       <c r="K34" t="n">
-        <v>-2</v>
+        <v>-4</v>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>⮟ -2</t>
+          <t>⮟ -4</t>
         </is>
       </c>
     </row>
@@ -2417,17 +2417,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>159.9</t>
+          <t>143.9</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>179.9 n/c</t>
+          <t>170.9 ⮟ -3</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>219.9 n/c</t>
+          <t>215.9 ⮟ -4</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -2451,19 +2451,19 @@
         </is>
       </c>
       <c r="I35" t="n">
-        <v>1.6</v>
+        <v>1.44</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K35" t="n">
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -6</t>
         </is>
       </c>
     </row>
@@ -2475,17 +2475,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>172.9</t>
+          <t>165.9</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>196.9 ⮟ -2</t>
+          <t>187.9 ⮟ -6</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>214.9 ⮟ -2</t>
+          <t>202.9 ⮟ -2</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -2509,7 +2509,7 @@
         </is>
       </c>
       <c r="I36" t="n">
-        <v>1.73</v>
+        <v>1.66</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -2517,11 +2517,11 @@
         </is>
       </c>
       <c r="K36" t="n">
-        <v>-2</v>
+        <v>-6</v>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>⮟ -2</t>
+          <t>⮟ -6</t>
         </is>
       </c>
     </row>
@@ -2533,17 +2533,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>152.9</t>
+          <t>146.9</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>182.9 ⮟ -5</t>
+          <t>176.9 ⮟ -6</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>197.9 ⮟ -2</t>
+          <t>191.9 ⮟ -4</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -2567,7 +2567,7 @@
         </is>
       </c>
       <c r="I37" t="n">
-        <v>1.53</v>
+        <v>1.47</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -2575,11 +2575,11 @@
         </is>
       </c>
       <c r="K37" t="n">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>⮟ -5</t>
+          <t>⮟ -6</t>
         </is>
       </c>
     </row>
@@ -2591,17 +2591,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>152.9</t>
+          <t>146.9</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>182.9 ⮟ -5</t>
+          <t>176.9 ⮟ -6</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>197.9 ⮟ -2</t>
+          <t>191.9 ⮟ -4</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -2625,7 +2625,7 @@
         </is>
       </c>
       <c r="I38" t="n">
-        <v>1.53</v>
+        <v>1.47</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -2633,11 +2633,11 @@
         </is>
       </c>
       <c r="K38" t="n">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>⮟ -5</t>
+          <t>⮟ -6</t>
         </is>
       </c>
     </row>
@@ -2649,17 +2649,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>162.9</t>
+          <t>151.9</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>180.9 n/c</t>
+          <t>169.9 ⮟ -6</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>196.9 n/c</t>
+          <t>191.9 ⮟ -5</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -2683,19 +2683,19 @@
         </is>
       </c>
       <c r="I39" t="n">
-        <v>1.63</v>
+        <v>1.52</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K39" t="n">
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -6</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
color update / text update
</commit_message>
<xml_diff>
--- a/data/tomorrow_gasprices_canadiancities_latlng.xlsx
+++ b/data/tomorrow_gasprices_canadiancities_latlng.xlsx
@@ -503,17 +503,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>146.9</t>
+          <t>142.9</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>176.9 n/c</t>
+          <t>172.9 ⮟ -4</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>191.9 n/c</t>
+          <t>195.9 ⮝ 4</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -537,19 +537,19 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>1.47</v>
+        <v>1.43</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -4</t>
         </is>
       </c>
     </row>
@@ -561,17 +561,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>161.9</t>
+          <t>157.9</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>185.9 n/c</t>
+          <t>181.9 ⮟ -4</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>215.9 n/c</t>
+          <t>219.9 ⮝ 4</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -595,19 +595,19 @@
         </is>
       </c>
       <c r="I3" t="n">
-        <v>1.62</v>
+        <v>1.58</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -4</t>
         </is>
       </c>
     </row>
@@ -619,7 +619,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>163.9</t>
+          <t>158.9</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -629,7 +629,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>216.9 n/c</t>
+          <t>218.9 ⮝ 2</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -653,19 +653,19 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>1.64</v>
+        <v>1.59</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -5</t>
         </is>
       </c>
     </row>
@@ -677,17 +677,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>127.9</t>
+          <t>125.9</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>152.9 n/c</t>
+          <t>150.9 ⮟ -2</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>172.9 n/c</t>
+          <t>174.9 ⮝ 2</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -711,19 +711,19 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>1.28</v>
+        <v>1.26</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -2</t>
         </is>
       </c>
     </row>
@@ -735,17 +735,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>145.9</t>
+          <t>141.9</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>175.9 n/c</t>
+          <t>171.9 ⮟ -4</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>191.9 n/c</t>
+          <t>195.9 ⮝ 4</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -769,19 +769,19 @@
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1.46</v>
+        <v>1.42</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -4</t>
         </is>
       </c>
     </row>
@@ -793,17 +793,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>146.9</t>
+          <t>142.9</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>176.9 n/c</t>
+          <t>172.9 ⮟ -4</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>191.9 n/c</t>
+          <t>195.9 ⮝ 4</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -827,19 +827,19 @@
         </is>
       </c>
       <c r="I7" t="n">
-        <v>1.47</v>
+        <v>1.43</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -4</t>
         </is>
       </c>
     </row>
@@ -909,12 +909,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>148.9</t>
+          <t>146.9</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>174.9 n/c</t>
+          <t>172.9 ⮟ -2</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -943,19 +943,19 @@
         </is>
       </c>
       <c r="I9" t="n">
-        <v>1.49</v>
+        <v>1.47</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -2</t>
         </is>
       </c>
     </row>
@@ -967,12 +967,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>125.9</t>
+          <t>123.9</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>153.9 n/c</t>
+          <t>151.9 ⮟ -2</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1001,19 +1001,19 @@
         </is>
       </c>
       <c r="I10" t="n">
-        <v>1.26</v>
+        <v>1.24</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -2</t>
         </is>
       </c>
     </row>
@@ -1083,17 +1083,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>146.9</t>
+          <t>142.9</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>176.9 n/c</t>
+          <t>172.9 ⮟ -4</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>191.9 n/c</t>
+          <t>195.9 ⮝ 4</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1117,19 +1117,19 @@
         </is>
       </c>
       <c r="I12" t="n">
-        <v>1.47</v>
+        <v>1.43</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -4</t>
         </is>
       </c>
     </row>
@@ -1199,17 +1199,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>146.9</t>
+          <t>142.9</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>176.9 n/c</t>
+          <t>172.9 ⮟ -4</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>191.9 n/c</t>
+          <t>195.9 ⮝ 4</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1233,19 +1233,19 @@
         </is>
       </c>
       <c r="I14" t="n">
-        <v>1.47</v>
+        <v>1.43</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -4</t>
         </is>
       </c>
     </row>
@@ -1257,17 +1257,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>165.9</t>
+          <t>163.9</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>187.9 n/c</t>
+          <t>185.9 ⮟ -2</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>201.9 n/c</t>
+          <t>199.9 ⮟ -2</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1291,19 +1291,19 @@
         </is>
       </c>
       <c r="I15" t="n">
-        <v>1.66</v>
+        <v>1.64</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -2</t>
         </is>
       </c>
     </row>
@@ -1315,17 +1315,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>165.9</t>
+          <t>163.9</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>187.9 n/c</t>
+          <t>185.9 ⮟ -2</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>201.9 n/c</t>
+          <t>199.9 ⮟ -2</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1349,19 +1349,19 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>1.66</v>
+        <v>1.64</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K16" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -2</t>
         </is>
       </c>
     </row>
@@ -1373,17 +1373,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>146.9</t>
+          <t>142.9</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>168.9 n/c</t>
+          <t>166.9 ⮟ -2</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>198.9 n/c</t>
+          <t>200.9 ⮝ 2</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1407,19 +1407,19 @@
         </is>
       </c>
       <c r="I17" t="n">
-        <v>1.47</v>
+        <v>1.43</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -4</t>
         </is>
       </c>
     </row>
@@ -1431,17 +1431,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>145.9</t>
+          <t>141.9</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>175.9 n/c</t>
+          <t>171.9 ⮟ -4</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>191.9 n/c</t>
+          <t>195.9 ⮝ 4</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1465,19 +1465,19 @@
         </is>
       </c>
       <c r="I18" t="n">
-        <v>1.46</v>
+        <v>1.42</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K18" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -4</t>
         </is>
       </c>
     </row>
@@ -1489,17 +1489,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>146.9</t>
+          <t>142.9</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>176.9 n/c</t>
+          <t>172.9 ⮟ -4</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>191.9 n/c</t>
+          <t>195.9 ⮝ 4</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1523,19 +1523,19 @@
         </is>
       </c>
       <c r="I19" t="n">
-        <v>1.47</v>
+        <v>1.43</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -4</t>
         </is>
       </c>
     </row>
@@ -1547,17 +1547,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>146.9</t>
+          <t>142.9</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>176.9 n/c</t>
+          <t>172.9 ⮟ -4</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>191.9 n/c</t>
+          <t>195.9 ⮝ 4</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1581,19 +1581,19 @@
         </is>
       </c>
       <c r="I20" t="n">
-        <v>1.47</v>
+        <v>1.43</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K20" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -4</t>
         </is>
       </c>
     </row>
@@ -1663,17 +1663,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>146.9</t>
+          <t>142.9</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>176.9 n/c</t>
+          <t>172.9 ⮟ -4</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>191.9 n/c</t>
+          <t>195.9 ⮝ 4</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1697,19 +1697,19 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>1.47</v>
+        <v>1.43</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K22" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -4</t>
         </is>
       </c>
     </row>
@@ -1721,17 +1721,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>146.9</t>
+          <t>142.9</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>176.9 n/c</t>
+          <t>172.9 ⮟ -4</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>191.9 n/c</t>
+          <t>195.9 ⮝ 4</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1755,19 +1755,19 @@
         </is>
       </c>
       <c r="I23" t="n">
-        <v>1.47</v>
+        <v>1.43</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K23" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -4</t>
         </is>
       </c>
     </row>
@@ -1779,17 +1779,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>145.9</t>
+          <t>141.9</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>175.9 n/c</t>
+          <t>172.9 ⮟ -3</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>191.9 n/c</t>
+          <t>195.9 ⮝ 4</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1813,19 +1813,19 @@
         </is>
       </c>
       <c r="I24" t="n">
-        <v>1.46</v>
+        <v>1.42</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K24" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -4</t>
         </is>
       </c>
     </row>
@@ -1837,17 +1837,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>146.9</t>
+          <t>142.9</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>193.9 n/c</t>
+          <t>172.9 ⮟ -21</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>204.9 n/c</t>
+          <t>201.9 ⮟ -3</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1871,19 +1871,19 @@
         </is>
       </c>
       <c r="I25" t="n">
-        <v>1.47</v>
+        <v>1.43</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K25" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -4</t>
         </is>
       </c>
     </row>
@@ -1895,17 +1895,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>139.9</t>
+          <t>137.9</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>164.9 n/c</t>
+          <t>162.9 ⮟ -2</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>196.9 n/c</t>
+          <t>198.9 ⮝ 2</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1929,19 +1929,19 @@
         </is>
       </c>
       <c r="I26" t="n">
-        <v>1.4</v>
+        <v>1.38</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K26" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -2</t>
         </is>
       </c>
     </row>
@@ -2011,12 +2011,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>166.9</t>
+          <t>162.9</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>187.9 n/c</t>
+          <t>184.9 ⮟ -3</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2045,19 +2045,19 @@
         </is>
       </c>
       <c r="I28" t="n">
-        <v>1.67</v>
+        <v>1.63</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K28" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -4</t>
         </is>
       </c>
     </row>
@@ -2069,12 +2069,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>147.9</t>
+          <t>143.9</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>170.9 n/c</t>
+          <t>167.9 ⮟ -3</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2103,19 +2103,19 @@
         </is>
       </c>
       <c r="I29" t="n">
-        <v>1.48</v>
+        <v>1.44</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K29" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -4</t>
         </is>
       </c>
     </row>
@@ -2127,12 +2127,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>147.9</t>
+          <t>143.9</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>170.9 n/c</t>
+          <t>167.9 ⮟ -3</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2161,19 +2161,19 @@
         </is>
       </c>
       <c r="I30" t="n">
-        <v>1.48</v>
+        <v>1.44</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K30" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -4</t>
         </is>
       </c>
     </row>
@@ -2185,17 +2185,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>146.9</t>
+          <t>142.9</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>176.9 n/c</t>
+          <t>172.9 ⮟ -4</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>191.9 n/c</t>
+          <t>195.9 ⮝ 4</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -2219,19 +2219,19 @@
         </is>
       </c>
       <c r="I31" t="n">
-        <v>1.47</v>
+        <v>1.43</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K31" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -4</t>
         </is>
       </c>
     </row>
@@ -2359,12 +2359,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>155.9</t>
+          <t>151.9</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>182.9 n/c</t>
+          <t>178.9 ⮟ -4</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2393,19 +2393,19 @@
         </is>
       </c>
       <c r="I34" t="n">
-        <v>1.56</v>
+        <v>1.52</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K34" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -4</t>
         </is>
       </c>
     </row>
@@ -2417,12 +2417,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>143.9</t>
+          <t>140.9</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>170.9 n/c</t>
+          <t>167.9 ⮟ -3</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -2451,19 +2451,19 @@
         </is>
       </c>
       <c r="I35" t="n">
-        <v>1.44</v>
+        <v>1.41</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K35" t="n">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -3</t>
         </is>
       </c>
     </row>
@@ -2475,12 +2475,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>165.9</t>
+          <t>160.9</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>187.9 n/c</t>
+          <t>182.9 ⮟ -5</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -2509,19 +2509,19 @@
         </is>
       </c>
       <c r="I36" t="n">
-        <v>1.66</v>
+        <v>1.61</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K36" t="n">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -5</t>
         </is>
       </c>
     </row>
@@ -2533,17 +2533,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>146.9</t>
+          <t>142.9</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>176.9 n/c</t>
+          <t>172.9 ⮟ -4</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>191.9 n/c</t>
+          <t>195.9 ⮝ 4</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -2567,19 +2567,19 @@
         </is>
       </c>
       <c r="I37" t="n">
-        <v>1.47</v>
+        <v>1.43</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K37" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -4</t>
         </is>
       </c>
     </row>
@@ -2591,17 +2591,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>146.9</t>
+          <t>142.9</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>176.9 n/c</t>
+          <t>172.9 ⮟ -4</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>191.9 n/c</t>
+          <t>195.9 ⮝ 4</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -2625,19 +2625,19 @@
         </is>
       </c>
       <c r="I38" t="n">
-        <v>1.47</v>
+        <v>1.43</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K38" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -4</t>
         </is>
       </c>
     </row>
@@ -2649,12 +2649,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>151.9</t>
+          <t>147.9</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>169.9 n/c</t>
+          <t>165.9 ⮟ -4</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -2683,19 +2683,19 @@
         </is>
       </c>
       <c r="I39" t="n">
-        <v>1.52</v>
+        <v>1.48</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K39" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -4</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
date and .csv update for historical gas prices across canada
</commit_message>
<xml_diff>
--- a/data/tomorrow_gasprices_canadiancities_latlng.xlsx
+++ b/data/tomorrow_gasprices_canadiancities_latlng.xlsx
@@ -503,17 +503,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>134.9</t>
+          <t>145.9</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>164.9 n/c</t>
+          <t>175.9 ⮟ -1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>201.9 n/c</t>
+          <t>210.9 n/c</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -537,19 +537,19 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>1.35</v>
+        <v>1.46</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -1</t>
         </is>
       </c>
     </row>
@@ -561,17 +561,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>150.9</t>
+          <t>161.9</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>180.9 n/c</t>
+          <t>191.9 ⮟ -1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>220.9 n/c</t>
+          <t>230.9 n/c</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -595,19 +595,19 @@
         </is>
       </c>
       <c r="I3" t="n">
-        <v>1.51</v>
+        <v>1.62</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -1</t>
         </is>
       </c>
     </row>
@@ -619,17 +619,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>161.9</t>
+          <t>170.9</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>190.9 n/c</t>
+          <t>199.9 n/c</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>209.9 n/c</t>
+          <t>229.9 n/c</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -653,7 +653,7 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>1.62</v>
+        <v>1.71</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -677,17 +677,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>122.9</t>
+          <t>118.9</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>147.9 n/c</t>
+          <t>142.9 ⮝ 7</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>172.9 n/c</t>
+          <t>176.9 n/c</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -711,19 +711,19 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>1.23</v>
+        <v>1.19</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮝</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮝ 7</t>
         </is>
       </c>
     </row>
@@ -735,17 +735,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>133.9</t>
+          <t>144.9</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>164.9 n/c</t>
+          <t>174.9 ⮟ -1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>201.9 n/c</t>
+          <t>210.9 n/c</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -769,19 +769,19 @@
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1.34</v>
+        <v>1.45</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -1</t>
         </is>
       </c>
     </row>
@@ -793,17 +793,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>134.9</t>
+          <t>145.9</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>164.9 n/c</t>
+          <t>175.9 ⮟ -1</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>201.9 n/c</t>
+          <t>210.9 n/c</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -827,19 +827,19 @@
         </is>
       </c>
       <c r="I7" t="n">
-        <v>1.35</v>
+        <v>1.46</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -1</t>
         </is>
       </c>
     </row>
@@ -851,17 +851,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>153.1</t>
+          <t>156.5</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>162.2 n/c</t>
+          <t>165.6 ⮝ 6</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>256.0 n/c</t>
+          <t>226.4 ⮝ 3</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -885,19 +885,19 @@
         </is>
       </c>
       <c r="I8" t="n">
-        <v>1.53</v>
+        <v>1.56</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮝</t>
         </is>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮝ 6</t>
         </is>
       </c>
     </row>
@@ -909,17 +909,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>134.9</t>
+          <t>145.9</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>160.9 n/c</t>
+          <t>165.9 ⮟ -1</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>203.9 n/c</t>
+          <t>214.9 n/c</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -943,19 +943,19 @@
         </is>
       </c>
       <c r="I9" t="n">
-        <v>1.35</v>
+        <v>1.46</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -1</t>
         </is>
       </c>
     </row>
@@ -967,17 +967,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>120.9</t>
+          <t>116.9</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>144.9 n/c</t>
+          <t>133.9 n/c</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>170.9 n/c</t>
+          <t>173.9 n/c</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1001,7 +1001,7 @@
         </is>
       </c>
       <c r="I10" t="n">
-        <v>1.21</v>
+        <v>1.17</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1025,17 +1025,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>146.9</t>
+          <t>154.4</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>154.6 n/c</t>
+          <t>161.7 n/c</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>210.3 n/c</t>
+          <t>209.2 n/c</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1059,7 +1059,7 @@
         </is>
       </c>
       <c r="I11" t="n">
-        <v>1.47</v>
+        <v>1.54</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1083,17 +1083,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>134.9</t>
+          <t>145.9</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>164.9 n/c</t>
+          <t>175.9 ⮟ -1</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>201.9 n/c</t>
+          <t>210.9 n/c</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1117,19 +1117,19 @@
         </is>
       </c>
       <c r="I12" t="n">
-        <v>1.35</v>
+        <v>1.46</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -1</t>
         </is>
       </c>
     </row>
@@ -1141,17 +1141,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>145.9</t>
+          <t>147.7</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>152.9 n/c</t>
+          <t>157.9 ⮝ 7</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>238.5 n/c</t>
+          <t>203.0 ⮝ 3</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1175,19 +1175,19 @@
         </is>
       </c>
       <c r="I13" t="n">
-        <v>1.46</v>
+        <v>1.48</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮝</t>
         </is>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮝ 6</t>
         </is>
       </c>
     </row>
@@ -1199,17 +1199,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>134.9</t>
+          <t>145.9</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>164.9 n/c</t>
+          <t>175.9 ⮟ -1</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>201.9 n/c</t>
+          <t>210.9 n/c</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1233,19 +1233,19 @@
         </is>
       </c>
       <c r="I14" t="n">
-        <v>1.35</v>
+        <v>1.46</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -1</t>
         </is>
       </c>
     </row>
@@ -1257,17 +1257,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>165.9</t>
+          <t>152.9</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>187.9 n/c</t>
+          <t>181.9 n/c</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>206.9 n/c</t>
+          <t>200.9 n/c</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1291,7 +1291,7 @@
         </is>
       </c>
       <c r="I15" t="n">
-        <v>1.66</v>
+        <v>1.53</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1315,17 +1315,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>165.9</t>
+          <t>145.9</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>187.9 n/c</t>
+          <t>167.9 n/c</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>206.9 n/c</t>
+          <t>200.9 n/c</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1349,7 +1349,7 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>1.66</v>
+        <v>1.46</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1373,17 +1373,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>134.9</t>
+          <t>145.9</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>165.9 n/c</t>
+          <t>167.9 ⮟ -1</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>212.9 n/c</t>
+          <t>216.9 n/c</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1407,19 +1407,19 @@
         </is>
       </c>
       <c r="I17" t="n">
-        <v>1.35</v>
+        <v>1.46</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -1</t>
         </is>
       </c>
     </row>
@@ -1431,17 +1431,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>133.9</t>
+          <t>144.9</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>163.9 n/c</t>
+          <t>174.9 ⮟ -1</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>201.9 n/c</t>
+          <t>210.9 n/c</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1465,19 +1465,19 @@
         </is>
       </c>
       <c r="I18" t="n">
-        <v>1.34</v>
+        <v>1.45</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K18" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -1</t>
         </is>
       </c>
     </row>
@@ -1489,17 +1489,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>134.9</t>
+          <t>145.9</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>164.9 n/c</t>
+          <t>175.9 ⮟ -1</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>201.9 n/c</t>
+          <t>210.9 n/c</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1523,19 +1523,19 @@
         </is>
       </c>
       <c r="I19" t="n">
-        <v>1.35</v>
+        <v>1.46</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -1</t>
         </is>
       </c>
     </row>
@@ -1547,17 +1547,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>134.9</t>
+          <t>145.9</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>164.9 n/c</t>
+          <t>175.9 ⮟ -1</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>201.9 n/c</t>
+          <t>210.9 n/c</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1581,19 +1581,19 @@
         </is>
       </c>
       <c r="I20" t="n">
-        <v>1.35</v>
+        <v>1.46</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K20" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -1</t>
         </is>
       </c>
     </row>
@@ -1605,17 +1605,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>147.6</t>
+          <t>152.9</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>155.3 n/c</t>
+          <t>161.8 n/c</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>260.3 n/c</t>
+          <t>209.2 n/c</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1639,7 +1639,7 @@
         </is>
       </c>
       <c r="I21" t="n">
-        <v>1.48</v>
+        <v>1.53</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1663,17 +1663,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>134.9</t>
+          <t>145.9</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>164.9 n/c</t>
+          <t>175.9 ⮟ -1</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>201.9 n/c</t>
+          <t>210.9 n/c</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1697,19 +1697,19 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>1.35</v>
+        <v>1.46</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K22" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -1</t>
         </is>
       </c>
     </row>
@@ -1721,17 +1721,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>134.9</t>
+          <t>145.9</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>164.9 n/c</t>
+          <t>175.9 ⮟ -1</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>201.9 n/c</t>
+          <t>210.9 n/c</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1755,19 +1755,19 @@
         </is>
       </c>
       <c r="I23" t="n">
-        <v>1.35</v>
+        <v>1.46</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K23" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -1</t>
         </is>
       </c>
     </row>
@@ -1779,17 +1779,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>133.9</t>
+          <t>144.9</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>163.9 n/c</t>
+          <t>174.9 ⮟ -1</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>201.9 n/c</t>
+          <t>210.9 n/c</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1813,19 +1813,19 @@
         </is>
       </c>
       <c r="I24" t="n">
-        <v>1.34</v>
+        <v>1.45</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K24" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -1</t>
         </is>
       </c>
     </row>
@@ -1837,17 +1837,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>134.9</t>
+          <t>145.9</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>164.9 n/c</t>
+          <t>175.9 ⮟ -1</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>214.9 n/c</t>
+          <t>222.9 n/c</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1871,19 +1871,19 @@
         </is>
       </c>
       <c r="I25" t="n">
-        <v>1.35</v>
+        <v>1.46</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K25" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -1</t>
         </is>
       </c>
     </row>
@@ -1900,12 +1900,12 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>153.9 n/c</t>
+          <t>154.9 ⮟ -1</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>196.9 n/c</t>
+          <t>211.9 n/c</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1933,15 +1933,15 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K26" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -1</t>
         </is>
       </c>
     </row>
@@ -1953,17 +1953,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>159.9</t>
+          <t>152.9</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>180.9 n/c</t>
+          <t>174.9 n/c</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>194.9 n/c</t>
+          <t>188.9 n/c</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1987,7 +1987,7 @@
         </is>
       </c>
       <c r="I27" t="n">
-        <v>1.6</v>
+        <v>1.53</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2011,17 +2011,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>154.9</t>
+          <t>160.9</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>177.9 n/c</t>
+          <t>181.9 ⮟ -1</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>220.9 n/c</t>
+          <t>234.9 n/c</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -2045,19 +2045,19 @@
         </is>
       </c>
       <c r="I28" t="n">
-        <v>1.55</v>
+        <v>1.61</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K28" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -1</t>
         </is>
       </c>
     </row>
@@ -2069,17 +2069,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>145.9</t>
+          <t>137.9</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>169.9 n/c</t>
+          <t>161.9 n/c</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>199.9 n/c</t>
+          <t>189.9 n/c</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -2103,7 +2103,7 @@
         </is>
       </c>
       <c r="I29" t="n">
-        <v>1.46</v>
+        <v>1.38</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2127,12 +2127,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>137.9</t>
+          <t>136.9</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>160.9 n/c</t>
+          <t>157.9 n/c</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2161,7 +2161,7 @@
         </is>
       </c>
       <c r="I30" t="n">
-        <v>1.38</v>
+        <v>1.37</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2185,17 +2185,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>134.9</t>
+          <t>145.9</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>164.9 n/c</t>
+          <t>175.9 ⮟ -1</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>201.9 n/c</t>
+          <t>210.9 n/c</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -2219,19 +2219,19 @@
         </is>
       </c>
       <c r="I31" t="n">
-        <v>1.35</v>
+        <v>1.46</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K31" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -1</t>
         </is>
       </c>
     </row>
@@ -2243,17 +2243,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>147.6</t>
+          <t>154.6</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>155.4 n/c</t>
+          <t>162.4 n/c</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>260.3 n/c</t>
+          <t>209.2 n/c</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -2277,7 +2277,7 @@
         </is>
       </c>
       <c r="I32" t="n">
-        <v>1.48</v>
+        <v>1.55</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -2301,7 +2301,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>162.9</t>
+          <t>162.6</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -2311,7 +2311,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>257.7 n/c</t>
+          <t>223.9 n/c</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -2359,17 +2359,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>144.9</t>
+          <t>129.9</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>172.9 n/c</t>
+          <t>178.9 n/c</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>199.9 n/c</t>
+          <t>212.9 n/c</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -2393,7 +2393,7 @@
         </is>
       </c>
       <c r="I34" t="n">
-        <v>1.45</v>
+        <v>1.3</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -2422,12 +2422,12 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>168.9 n/c</t>
+          <t>182.9 n/c</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>219.9 n/c</t>
+          <t>217.9 n/c</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -2475,17 +2475,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>162.9</t>
+          <t>155.9</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>183.9 n/c</t>
+          <t>179.9 n/c</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>182.9 n/c</t>
+          <t>185.9 n/c</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -2509,7 +2509,7 @@
         </is>
       </c>
       <c r="I36" t="n">
-        <v>1.63</v>
+        <v>1.56</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -2533,17 +2533,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>134.9</t>
+          <t>145.9</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>164.9 n/c</t>
+          <t>175.9 ⮟ -1</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>201.9 n/c</t>
+          <t>210.9 n/c</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -2567,19 +2567,19 @@
         </is>
       </c>
       <c r="I37" t="n">
-        <v>1.35</v>
+        <v>1.46</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K37" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -1</t>
         </is>
       </c>
     </row>
@@ -2591,17 +2591,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>134.9</t>
+          <t>145.9</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>164.9 n/c</t>
+          <t>175.9 ⮟ -1</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>201.9 n/c</t>
+          <t>210.9 n/c</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -2625,19 +2625,19 @@
         </is>
       </c>
       <c r="I38" t="n">
-        <v>1.35</v>
+        <v>1.46</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟</t>
         </is>
       </c>
       <c r="K38" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>n/c</t>
+          <t>⮟ -1</t>
         </is>
       </c>
     </row>
@@ -2649,12 +2649,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>152.9</t>
+          <t>147.9</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>170.9 n/c</t>
+          <t>165.9 n/c</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -2683,7 +2683,7 @@
         </is>
       </c>
       <c r="I39" t="n">
-        <v>1.53</v>
+        <v>1.48</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>

</xml_diff>